<commit_message>
Supression de compte faite
</commit_message>
<xml_diff>
--- a/Documentation/03a - DescriptionProduit.xlsx
+++ b/Documentation/03a - DescriptionProduit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Documents\GitHub\symmetrical-guacamole\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACE87E3-8F6B-4D6F-AAC6-545BF8FC1760}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23AEB03-392D-47E3-AE0D-0E1279CAD042}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -301,13 +301,13 @@
     <t>FAIT</t>
   </si>
   <si>
-    <t>Mettre un credit de 100 points</t>
-  </si>
-  <si>
     <t>Faire les filtres</t>
   </si>
   <si>
     <t>Faire la page creer un article</t>
+  </si>
+  <si>
+    <t>Il faut creer une page profil  pour utilisateur different</t>
   </si>
 </sst>
 </file>
@@ -458,9 +458,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -493,6 +490,9 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,48 +851,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="6" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -920,334 +920,335 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+    <row r="7" spans="1:8" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
         <v>1</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>2000</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>1001</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+    <row r="8" spans="1:8" s="15" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
         <v>1</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="12">
         <v>1900</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="12">
         <v>1003</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>1</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1800</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="12">
+        <v>6002</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>1</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1750</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1009</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>1</v>
+      </c>
+      <c r="B11" s="16">
+        <v>1700</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1006</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1600</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1007</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>1</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1500</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1004</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>1</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1400</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="16">
+        <v>2001</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>1</v>
+      </c>
+      <c r="B15" s="16">
+        <v>1300</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="16">
+        <v>2004</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+    <row r="16" spans="1:8" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
         <v>1</v>
       </c>
-      <c r="B9" s="13">
-        <v>1800</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="B16" s="16">
+        <v>1200</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="16">
+        <v>2005</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="23" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>1</v>
+      </c>
+      <c r="B17" s="20">
+        <v>1100</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="20">
+        <v>2006</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" s="23" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <v>1</v>
+      </c>
+      <c r="B18" s="20">
+        <v>1000</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="20">
+        <v>2007</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" s="15" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>1</v>
+      </c>
+      <c r="B19" s="12">
+        <v>950</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="13">
-        <v>6002</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="D19" s="12">
+        <v>6003</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
         <v>1</v>
       </c>
-      <c r="B10" s="17">
-        <v>1750</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="17">
-        <v>1009</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="19"/>
-    </row>
-    <row r="11" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="B20" s="12">
+        <v>900</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="12">
+        <v>2009</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
         <v>1</v>
       </c>
-      <c r="B11" s="17">
-        <v>1700</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="17">
-        <v>1006</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="19"/>
-    </row>
-    <row r="12" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>1</v>
-      </c>
-      <c r="B12" s="17">
-        <v>1600</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="17">
-        <v>1007</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="1:8" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>1</v>
-      </c>
-      <c r="B13" s="17">
-        <v>1500</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="17">
-        <v>1004</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
-        <v>1</v>
-      </c>
-      <c r="B14" s="17">
-        <v>1400</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="17">
-        <v>2001</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
-        <v>1</v>
-      </c>
-      <c r="B15" s="17">
-        <v>1300</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="17">
-        <v>2004</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
-        <v>1</v>
-      </c>
-      <c r="B16" s="17">
-        <v>1200</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="17">
-        <v>2005</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="24" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
-        <v>1</v>
-      </c>
-      <c r="B17" s="21">
-        <v>1100</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="21">
-        <v>2006</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="23"/>
-    </row>
-    <row r="18" spans="1:8" s="24" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
-        <v>1</v>
-      </c>
-      <c r="B18" s="21">
-        <v>1000</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="21">
-        <v>2007</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="23"/>
-    </row>
-    <row r="19" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
-        <v>1</v>
-      </c>
-      <c r="B19" s="13">
-        <v>950</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="B21" s="12">
+        <v>850</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="13">
-        <v>6003</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:8" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
-        <v>1</v>
-      </c>
-      <c r="B20" s="13">
-        <v>900</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="13">
-        <v>2009</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8" s="24" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
-        <v>1</v>
-      </c>
-      <c r="B21" s="21">
-        <v>850</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="21">
+      <c r="D21" s="12">
         <v>6001</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23" t="s">
+      <c r="G21" s="14"/>
+      <c r="H21" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1272,27 +1273,27 @@
       </c>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:8" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23" spans="1:8" s="15" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
         <v>2</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="12">
         <v>750</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="12">
         <v>8001</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">

</xml_diff>

<commit_message>
Les pages utilisateurs autres crees
</commit_message>
<xml_diff>
--- a/Documentation/03a - DescriptionProduit.xlsx
+++ b/Documentation/03a - DescriptionProduit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Documents\GitHub\symmetrical-guacamole\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23AEB03-392D-47E3-AE0D-0E1279CAD042}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540FACC0-78C8-420F-BA54-B637F5CECECD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="90">
   <si>
     <t>ENI-ENCHERES</t>
   </si>
@@ -307,7 +307,7 @@
     <t>Faire la page creer un article</t>
   </si>
   <si>
-    <t>Il faut creer une page profil  pour utilisateur different</t>
+    <t>Creer un filtre , les utilisateurs non connectes ne doivent pas avoir acces aux pages profils deconnexion modifier etc</t>
   </si>
 </sst>
 </file>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,29 +1006,26 @@
       </c>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="11" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <v>1</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="12">
         <v>1700</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="12">
         <v>1006</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="19" t="s">
-        <v>89</v>
-      </c>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
@@ -1097,28 +1094,26 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+    <row r="15" spans="1:8" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
         <v>1</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="12">
         <v>1300</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="12">
         <v>2004</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="18" t="s">
-        <v>87</v>
-      </c>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:8" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
@@ -1228,7 +1223,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
     </row>
-    <row r="21" spans="1:8" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="15" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>1</v>
       </c>
@@ -1247,7 +1242,9 @@
       <c r="F21" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="14"/>
+      <c r="G21" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="H21" s="14" t="s">
         <v>44</v>
       </c>
@@ -1691,12 +1688,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1864,15 +1858,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{077AF987-EBAE-4C83-82B3-6D18035DFB9C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8E6F12F-7E5C-49A2-82AD-135EE890E1AF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1896,10 +1894,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8E6F12F-7E5C-49A2-82AD-135EE890E1AF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{077AF987-EBAE-4C83-82B3-6D18035DFB9C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Debut de la classe enchere
</commit_message>
<xml_diff>
--- a/Documentation/03a - DescriptionProduit.xlsx
+++ b/Documentation/03a - DescriptionProduit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Documents\GitHub\symmetrical-guacamole\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540FACC0-78C8-420F-BA54-B637F5CECECD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2C82E0-58E5-478E-ACAA-5CA77D0CD583}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
   <si>
     <t>ENI-ENCHERES</t>
   </si>
@@ -301,13 +301,19 @@
     <t>FAIT</t>
   </si>
   <si>
-    <t>Faire les filtres</t>
-  </si>
-  <si>
-    <t>Faire la page creer un article</t>
-  </si>
-  <si>
     <t>Creer un filtre , les utilisateurs non connectes ne doivent pas avoir acces aux pages profils deconnexion modifier etc</t>
+  </si>
+  <si>
+    <t>Il faut tout modifier a l'heure actuelle : il faudrait pouvoir change un champ a la fois</t>
+  </si>
+  <si>
+    <t>Pas compatible avec firefox</t>
+  </si>
+  <si>
+    <t>Faire les filtres encheres avec une offre et encheres gagnees ainsi que mes ventes</t>
+  </si>
+  <si>
+    <t>utiliser un listener</t>
   </si>
 </sst>
 </file>
@@ -833,7 +839,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,27 +1033,29 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+    <row r="12" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <v>1</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="16">
         <v>1600</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="16">
         <v>1007</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="G12" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
@@ -1071,27 +1079,27 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+    <row r="14" spans="1:8" s="15" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>1</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="12">
         <v>1400</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="12">
         <v>2001</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="14" t="s">
         <v>29</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1135,7 +1143,7 @@
         <v>33</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="23" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1178,7 +1186,9 @@
       <c r="F18" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="22"/>
+      <c r="G18" s="22" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="19" spans="1:8" s="15" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
@@ -1242,8 +1252,8 @@
       <c r="F21" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>89</v>
+      <c r="G21" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="H21" s="14" t="s">
         <v>44</v>
@@ -1688,9 +1698,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1858,19 +1871,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8E6F12F-7E5C-49A2-82AD-135EE890E1AF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{077AF987-EBAE-4C83-82B3-6D18035DFB9C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1894,9 +1903,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{077AF987-EBAE-4C83-82B3-6D18035DFB9C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8E6F12F-7E5C-49A2-82AD-135EE890E1AF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Quelques modifs, ajout du filter, changement de la bdd de base
</commit_message>
<xml_diff>
--- a/Documentation/03a - DescriptionProduit.xlsx
+++ b/Documentation/03a - DescriptionProduit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Val\Documents\GitHub\symmetrical-guacamole\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2C82E0-58E5-478E-ACAA-5CA77D0CD583}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D7E418-49E1-46CE-A785-244156422260}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="93">
   <si>
     <t>ENI-ENCHERES</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Creer un filtre , les utilisateurs non connectes ne doivent pas avoir acces aux pages profils deconnexion modifier etc</t>
   </si>
   <si>
-    <t>Il faut tout modifier a l'heure actuelle : il faudrait pouvoir change un champ a la fois</t>
-  </si>
-  <si>
     <t>Pas compatible avec firefox</t>
   </si>
   <si>
@@ -314,13 +311,19 @@
   </si>
   <si>
     <t>utiliser un listener</t>
+  </si>
+  <si>
+    <t>pas un upload</t>
+  </si>
+  <si>
+    <t>Il faut supprimer tous les articles lies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -349,20 +352,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,11 +386,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -427,13 +418,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,16 +464,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -494,17 +474,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -838,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,48 +839,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1033,29 +1015,27 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+    <row r="12" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>1</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="12">
         <v>1600</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="12">
         <v>1007</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="18"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
@@ -1099,7 +1079,7 @@
         <v>29</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1143,51 +1123,51 @@
         <v>33</v>
       </c>
       <c r="G16" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="15" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>1</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1100</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="12">
+        <v>2006</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" s="15" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>1</v>
+      </c>
+      <c r="B18" s="12">
+        <v>1000</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="12">
+        <v>2007</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="23" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
-        <v>1</v>
-      </c>
-      <c r="B17" s="20">
-        <v>1100</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="20">
-        <v>2006</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="22"/>
-    </row>
-    <row r="18" spans="1:8" s="23" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
-        <v>1</v>
-      </c>
-      <c r="B18" s="20">
-        <v>1000</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="20">
-        <v>2007</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="15" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1302,27 +1282,26 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24" spans="1:8" s="15" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
         <v>2</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="12">
         <v>700</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="12">
         <v>1002</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:8" s="9" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -1367,46 +1346,51 @@
       </c>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27" spans="1:8" s="19" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
         <v>2</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="16">
         <v>600</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="16">
         <v>2008</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="G27" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="19" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
         <v>2</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="16">
         <v>500</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="16">
         <v>3001</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="G28" s="10"/>
+      <c r="G28" s="18" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">

</xml_diff>